<commit_message>
fig login, import file
</commit_message>
<xml_diff>
--- a/PAKNAPI/Upload/BusinessIndividual/SampleFilesIndividual.xlsx
+++ b/PAKNAPI/Upload/BusinessIndividual/SampleFilesIndividual.xlsx
@@ -16,27 +16,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
-    <t>Công ty TNHHNN 1TV Thoát nước Hà Nội</t>
-  </si>
-  <si>
     <t>01/01/2018</t>
   </si>
   <si>
-    <t>Phòng khám đa khoa Quảng Tây</t>
-  </si>
-  <si>
     <t>02/01/2018</t>
   </si>
   <si>
-    <t>Bệnh viện tâm thần Mỹ Đức</t>
-  </si>
-  <si>
     <t>01/03/2018</t>
   </si>
   <si>
-    <t>Bệnh viện An Việt</t>
-  </si>
-  <si>
     <t>01/04/2018</t>
   </si>
   <si>
@@ -94,21 +82,12 @@
     <t>Khác</t>
   </si>
   <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
-    <t>2@gmail.com</t>
-  </si>
-  <si>
     <t>3@gmail.com</t>
   </si>
   <si>
@@ -119,6 +98,99 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Tên cá nhân </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Địa chỉ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngày sinh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <t>Trần Minh Trường</t>
+  </si>
+  <si>
+    <t>Trần Đình Hùng</t>
+  </si>
+  <si>
+    <t>Đinh Thị Loan</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Giới tính </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trạng thái </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CMND/CCCD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)(**)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Số điện thoại </t>
     </r>
     <r>
@@ -128,12 +200,76 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>(*)(**)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DANH SÁCH CÁ NHÂN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : Không được bỏ trống, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>(**)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CMND/CCCD </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : Không trùng lặp, Ngày tháng phải là định dạng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MM/dd/yyyy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email </t>
     </r>
     <r>
       <rPr>
@@ -146,138 +282,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Email </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(**)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tên cá nhân </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Địa chỉ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ngày sinh </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">DANH SÁCH CÁ NHÂN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : Không được bỏ trống, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(**)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : Không được bỏ trống và trùng lặp, Ngày tháng phải là định dạng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>dd/MM/yyyy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Quốc tịch </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
+    <t>Nguyễn Mạnh Hùng</t>
+  </si>
+  <si>
+    <t>Quốc tịch</t>
+  </si>
+  <si>
+    <t>Ngày cấp</t>
   </si>
 </sst>
 </file>
@@ -370,13 +381,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -679,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -691,241 +702,249 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" style="2" customWidth="1"/>
-    <col min="5" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" style="1" customWidth="1"/>
+    <col min="5" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+    <row r="1" spans="1:14" ht="30" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5">
         <v>32324232349</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="I3" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M3" s="3" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5">
         <v>32324232350</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
+      <c r="F4" s="7">
+        <v>44188</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="I4" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="3" t="b">
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="5">
         <v>32324232351</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="I5" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="3" t="b">
+      <c r="L5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="5" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5">
         <v>32324232352</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="3" t="b">
+      <c r="J6" s="5"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>